<commit_message>
update on extract code
</commit_message>
<xml_diff>
--- a/Pos_data_stat/position/top14-part2.xlsx
+++ b/Pos_data_stat/position/top14-part2.xlsx
@@ -457,16 +457,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7101</v>
+        <v>7088</v>
       </c>
       <c r="B2" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C2" t="n">
-        <v>2194</v>
+        <v>2208</v>
       </c>
       <c r="D2" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>